<commit_message>
test results in Excel
</commit_message>
<xml_diff>
--- a/src/main/resources/Excel.xlsx
+++ b/src/main/resources/Excel.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Imię</t>
   </si>
@@ -23,6 +23,9 @@
     <t>Pesel</t>
   </si>
   <si>
+    <t>Koronawirus</t>
+  </si>
+  <si>
     <t>posiadane pieniądze</t>
   </si>
   <si>
@@ -35,6 +38,9 @@
     <t>99087666341</t>
   </si>
   <si>
+    <t>brak</t>
+  </si>
+  <si>
     <t>Mikołaj</t>
   </si>
   <si>
@@ -51,6 +57,9 @@
   </si>
   <si>
     <t>82345678910</t>
+  </si>
+  <si>
+    <t>pozytywny</t>
   </si>
   <si>
     <t>Test</t>
@@ -98,7 +107,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -117,61 +126,76 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="n">
-        <v>123.0</v>
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="n">
+        <v>23.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="n">
-        <v>320.0</v>
+      <c r="E3" t="n">
+        <v>220.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="n">
-        <v>700.0</v>
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="n">
+        <v>100.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
       <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="n">
-        <v>123.0</v>
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="n">
+        <v>23.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>